<commit_message>
Se creo el primer escenario, con el tambien el step definition de dicho escenario
</commit_message>
<xml_diff>
--- a/DocumentaciónProyecto.xlsx
+++ b/DocumentaciónProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliana.perez\IdeaProjects\MyShopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70B1669F-260F-46CA-A2D2-4A31320810CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D538B27-3E13-46D2-BD87-296C3CC8A189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA8E4C43-C2B6-462E-8A59-DF9A5E3528B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nombre del escenario</t>
   </si>
@@ -54,6 +54,18 @@
   </si>
   <si>
     <t>RegistroUsuario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En la pagina de myShopify me registro como un nuevo usuario </t>
+  </si>
+  <si>
+    <t>Encontrarse en el formulario de registro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El usuario este registrado y en su nueva cuenta </t>
+  </si>
+  <si>
+    <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si registro mi usuario mirando mi perfil.</t>
   </si>
 </sst>
 </file>
@@ -115,11 +127,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -457,44 +475,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56013565-51B5-4BB7-B07D-5E35E87CC942}">
   <dimension ref="B3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="32.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:6" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
Se tuvieron que hacer cambios debido al capcha encontrado en la pagina, estos cambios fueron sobre el escenario cambiandolo un poco, terminamos este escenario y ahora esta listo y funcional
</commit_message>
<xml_diff>
--- a/DocumentaciónProyecto.xlsx
+++ b/DocumentaciónProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliana.perez\IdeaProjects\MyShopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D538B27-3E13-46D2-BD87-296C3CC8A189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1326B0A1-6DF4-49AC-83A3-F1998CC31232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA8E4C43-C2B6-462E-8A59-DF9A5E3528B5}"/>
   </bookViews>
@@ -53,19 +53,19 @@
     <t>Resultado esperado</t>
   </si>
   <si>
-    <t>RegistroUsuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En la pagina de myShopify me registro como un nuevo usuario </t>
-  </si>
-  <si>
     <t>Encontrarse en el formulario de registro.</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario este registrado y en su nueva cuenta </t>
-  </si>
-  <si>
-    <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si registro mi usuario mirando mi perfil.</t>
+    <t>No registra mi usuario y aparece el capcha para verificar que no es un robot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparicion de capcha </t>
+  </si>
+  <si>
+    <t>En la pagina de myShopify me intento registrar sin embargo el capcha no me deja debido a que es un robot</t>
+  </si>
+  <si>
+    <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si haya aprecido el capcha.</t>
   </si>
 </sst>
 </file>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56013565-51B5-4BB7-B07D-5E35E87CC942}">
   <dimension ref="B3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,19 +507,19 @@
     </row>
     <row r="4" spans="2:6" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se modifico la domentación, empezamos la preparación para el nuevo escenario
</commit_message>
<xml_diff>
--- a/DocumentaciónProyecto.xlsx
+++ b/DocumentaciónProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliana.perez\IdeaProjects\MyShopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D538B27-3E13-46D2-BD87-296C3CC8A189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF4C0A0-F8F1-4E4D-9B41-435DF9E17367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA8E4C43-C2B6-462E-8A59-DF9A5E3528B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nombre del escenario</t>
   </si>
@@ -53,19 +53,34 @@
     <t>Resultado esperado</t>
   </si>
   <si>
-    <t>RegistroUsuario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En la pagina de myShopify me registro como un nuevo usuario </t>
-  </si>
-  <si>
     <t>Encontrarse en el formulario de registro.</t>
   </si>
   <si>
-    <t xml:space="preserve">El usuario este registrado y en su nueva cuenta </t>
-  </si>
-  <si>
-    <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si registro mi usuario mirando mi perfil.</t>
+    <t>No registra mi usuario y aparece el capcha para verificar que no es un robot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aparicion de capcha </t>
+  </si>
+  <si>
+    <t>En la pagina de myShopify me intento registrar sin embargo el capcha no me deja debido a que es un robot</t>
+  </si>
+  <si>
+    <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si haya aprecido el capcha.</t>
+  </si>
+  <si>
+    <t>Buscar funcional</t>
+  </si>
+  <si>
+    <t>En la pagina de myshopify en el home utilizo el buscador y me aparece un resultado relacionado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Me encuentro en el home </t>
+  </si>
+  <si>
+    <t>Me aparece un resultado parecido a lo que busque.</t>
+  </si>
+  <si>
+    <t>1. ingresar en el buscador  una palabra clave de algun articulo 2. ver el nombre de la primera opción y verificar que si contenga algo relaciónado con la palabra clave ingresada</t>
   </si>
 </sst>
 </file>
@@ -127,9 +142,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,7 +490,7 @@
   <dimension ref="B3:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,45 +503,55 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+    </row>
+    <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>

</xml_diff>

<commit_message>
Se realizo un nuevo escenario relacionado con el home, se termino debido a que solo se tenia qque declarar algo en especifico, escenario listo
</commit_message>
<xml_diff>
--- a/DocumentaciónProyecto.xlsx
+++ b/DocumentaciónProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliana.perez\IdeaProjects\MyShopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF4C0A0-F8F1-4E4D-9B41-435DF9E17367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145592C3-C7F5-4E98-B8EE-4AA3477C6324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA8E4C43-C2B6-462E-8A59-DF9A5E3528B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nombre del escenario</t>
   </si>
@@ -62,18 +62,12 @@
     <t xml:space="preserve">Aparicion de capcha </t>
   </si>
   <si>
-    <t>En la pagina de myShopify me intento registrar sin embargo el capcha no me deja debido a que es un robot</t>
-  </si>
-  <si>
     <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si haya aprecido el capcha.</t>
   </si>
   <si>
     <t>Buscar funcional</t>
   </si>
   <si>
-    <t>En la pagina de myshopify en el home utilizo el buscador y me aparece un resultado relacionado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Me encuentro en el home </t>
   </si>
   <si>
@@ -81,6 +75,24 @@
   </si>
   <si>
     <t>1. ingresar en el buscador  una palabra clave de algun articulo 2. ver el nombre de la primera opción y verificar que si contenga algo relaciónado con la palabra clave ingresada</t>
+  </si>
+  <si>
+    <t>BusquedaFallida</t>
+  </si>
+  <si>
+    <t>En el portal de myshopify en el home utilizo el buscador y me aparece un resultado relacionado</t>
+  </si>
+  <si>
+    <t>En el portal de myShopify me intento registrar sin embargo el capcha no me deja debido a que es un robot</t>
+  </si>
+  <si>
+    <t>En el portal de myshopify utlizo el buscador con algo que no se encuentre en la tienda, debe aparecer el mensaje indicando que no hubieron resultados.</t>
+  </si>
+  <si>
+    <t>Me aparece el mensaje 'No results found for'</t>
+  </si>
+  <si>
+    <t>1. ingresar en el buscador  una palabra de algo que no se vende en la tienda. 2. verificar que se encuentre el mensaje que le avisa al usuario que no se encontraro resultados.</t>
   </si>
 </sst>
 </file>
@@ -490,7 +502,7 @@
   <dimension ref="B3:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +536,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>6</v>
@@ -538,27 +550,37 @@
     </row>
     <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
+    </row>
+    <row r="6" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
se actualizo el archivo de documentacion
</commit_message>
<xml_diff>
--- a/DocumentaciónProyecto.xlsx
+++ b/DocumentaciónProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliana.perez\IdeaProjects\MyShopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF4C0A0-F8F1-4E4D-9B41-435DF9E17367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380F7622-930C-49E7-AFED-AAA5A40FD3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA8E4C43-C2B6-462E-8A59-DF9A5E3528B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Nombre del escenario</t>
   </si>
@@ -62,18 +62,12 @@
     <t xml:space="preserve">Aparicion de capcha </t>
   </si>
   <si>
-    <t>En la pagina de myShopify me intento registrar sin embargo el capcha no me deja debido a que es un robot</t>
-  </si>
-  <si>
     <t>1. ir a la opcion del formulario de registro. 2. llenar los datos entregados para el registro en el formulario. 3. darle submit. 4. verifico que si haya aprecido el capcha.</t>
   </si>
   <si>
     <t>Buscar funcional</t>
   </si>
   <si>
-    <t>En la pagina de myshopify en el home utilizo el buscador y me aparece un resultado relacionado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Me encuentro en el home </t>
   </si>
   <si>
@@ -81,6 +75,24 @@
   </si>
   <si>
     <t>1. ingresar en el buscador  una palabra clave de algun articulo 2. ver el nombre de la primera opción y verificar que si contenga algo relaciónado con la palabra clave ingresada</t>
+  </si>
+  <si>
+    <t>BusquedaFallida</t>
+  </si>
+  <si>
+    <t>En el portal de myshopify en el home utilizo el buscador y me aparece un resultado relacionado</t>
+  </si>
+  <si>
+    <t>En el portal de myShopify me intento registrar sin embargo el capcha no me deja debido a que es un robot</t>
+  </si>
+  <si>
+    <t>En el portal de myshopify utlizo el buscador con algo que no se encuentre en la tienda, debe aparecer el mensaje indicando que no hubieron resultados.</t>
+  </si>
+  <si>
+    <t>Me aparece el mensaje 'No results found for'</t>
+  </si>
+  <si>
+    <t>1. ingresar en el buscador  una palabra de algo que no se vende en la tienda. 2. verificar que se encuentre el mensaje que le avisa al usuario que no se encontraro resultados.</t>
   </si>
 </sst>
 </file>
@@ -490,7 +502,7 @@
   <dimension ref="B3:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +536,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>6</v>
@@ -538,27 +550,37 @@
     </row>
     <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
+    </row>
+    <row r="6" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
Se documentaron los dos ultimos escenarios y se empezo con el nuevo feature
</commit_message>
<xml_diff>
--- a/DocumentaciónProyecto.xlsx
+++ b/DocumentaciónProyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eliana.perez\IdeaProjects\MyShopify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380F7622-930C-49E7-AFED-AAA5A40FD3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71B214D-CB04-4954-B841-C20C758B9844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{AA8E4C43-C2B6-462E-8A59-DF9A5E3528B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Nombre del escenario</t>
   </si>
@@ -93,6 +93,30 @@
   </si>
   <si>
     <t>1. ingresar en el buscador  una palabra de algo que no se vende en la tienda. 2. verificar que se encuentre el mensaje que le avisa al usuario que no se encontraro resultados.</t>
+  </si>
+  <si>
+    <t>AgregarArticulo</t>
+  </si>
+  <si>
+    <t>En el portal de myshopify agrego un articulo al carrito de compras</t>
+  </si>
+  <si>
+    <t>1. le doy click a la primera opción de los articulos 2. Cuando me manda a la información del articulo darle click al boton de agregar al carrito. 3. recargar la pagina 4. entrar al carrito.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El carrito tiene el articulo </t>
+  </si>
+  <si>
+    <t>EliminarArticulo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el portal de myshopify elimino un articulo del carroto de compras </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. le doy click a la primera opción de los articulos 2. Cuando me manda a la información del articulo darle click al boton de agregar al carrito. 3. recargar la pagina 4. entrar al carrito. 5. Elimino el articulo </t>
+  </si>
+  <si>
+    <t>El carrito esta vacio</t>
   </si>
 </sst>
 </file>
@@ -501,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56013565-51B5-4BB7-B07D-5E35E87CC942}">
   <dimension ref="B3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,19 +606,39 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+    <row r="7" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="8" spans="2:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>